<commit_message>
updated condiitons for none
</commit_message>
<xml_diff>
--- a/aoiConditions/train1P1Block10Test.xlsx
+++ b/aoiConditions/train1P1Block10Test.xlsx
@@ -22,7 +22,7 @@
     <t>imageTrue</t>
   </si>
   <si>
-    <t>audioFalse</t>
+    <t>currentPhase</t>
   </si>
   <si>
     <t>imageFalse</t>
@@ -40,7 +40,7 @@
     <t>pngimages/04_ladder.png</t>
   </si>
   <si>
-    <t>trainingaudio/21_papika1.wav</t>
+    <t>train1P1</t>
   </si>
   <si>
     <t>pngimages/21_cheese.png</t>

</xml_diff>